<commit_message>
Allow entering inventory value in inventory adjustment screen.
</commit_message>
<xml_diff>
--- a/test/integration/project/data_inventory.xlsx
+++ b/test/integration/project/data_inventory.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="270" windowWidth="14940" windowHeight="7575" activeTab="2"/>
+    <workbookView xWindow="360" yWindow="270" windowWidth="14940" windowHeight="7575" firstSheet="13" activeTab="16"/>
   </bookViews>
   <sheets>
     <sheet name="Supplier" sheetId="6" r:id="rId1"/>
@@ -26,15 +26,12 @@
     <sheet name="PenyesuaianStok_items" sheetId="17" r:id="rId17"/>
     <sheet name="Pesan" sheetId="19" r:id="rId18"/>
   </sheets>
-  <definedNames>
-    <definedName name="LOCAL_MYSQL_DATE_FORMAT" hidden="1">REPT(LOCAL_YEAR_FORMAT,4)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_MONTH_FORMAT,2)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_DAY_FORMAT,2)&amp;" "&amp;REPT(LOCAL_HOUR_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_MINUTE_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_SECOND_FORMAT,2)</definedName>
-  </definedNames>
   <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="302" uniqueCount="125">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="305" uniqueCount="127">
   <si>
     <t>id</t>
   </si>
@@ -409,13 +406,19 @@
   </si>
   <si>
     <t>jumlahTukar</t>
+  </si>
+  <si>
+    <t>createdBy</t>
+  </si>
+  <si>
+    <t>modifiedBy</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -425,13 +428,25 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFD7D7D7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -446,12 +461,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1958,41 +1974,60 @@
 
 <file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I1"/>
+  <dimension ref="A1:K1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I1" sqref="I1"/>
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="8" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="7.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="39.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="20.140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="7.85546875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="10.5703125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A1" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>111</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>125</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="F1" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="C1" t="s">
+      <c r="G1" s="5" t="s">
+        <v>126</v>
+      </c>
+      <c r="H1" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="I1" s="5" t="s">
         <v>58</v>
       </c>
-      <c r="D1" t="s">
+      <c r="J1" s="5" t="s">
         <v>60</v>
       </c>
-      <c r="E1" t="s">
-        <v>1</v>
-      </c>
-      <c r="F1" t="s">
-        <v>2</v>
-      </c>
-      <c r="G1" t="s">
-        <v>4</v>
-      </c>
-      <c r="H1" t="s">
+      <c r="K1" s="5" t="s">
         <v>18</v>
-      </c>
-      <c r="I1" t="s">
-        <v>111</v>
       </c>
     </row>
   </sheetData>
@@ -2003,25 +2038,33 @@
 
 <file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D1"/>
+  <dimension ref="A1:E1"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="19.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.42578125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A1" s="5" t="s">
         <v>110</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" s="5" t="s">
         <v>105</v>
       </c>
     </row>
@@ -2183,8 +2226,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O2" sqref="O2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F30" sqref="F30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Refactor move periodical aggregations to reusable abstract classes.
</commit_message>
<xml_diff>
--- a/test/integration/project/data_inventory.xlsx
+++ b/test/integration/project/data_inventory.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="270" windowWidth="14940" windowHeight="7575" firstSheet="13" activeTab="16"/>
+    <workbookView xWindow="360" yWindow="270" windowWidth="14940" windowHeight="7575" firstSheet="9" activeTab="12"/>
   </bookViews>
   <sheets>
     <sheet name="Supplier" sheetId="6" r:id="rId1"/>
@@ -26,12 +26,15 @@
     <sheet name="PenyesuaianStok_items" sheetId="17" r:id="rId17"/>
     <sheet name="Pesan" sheetId="19" r:id="rId18"/>
   </sheets>
+  <definedNames>
+    <definedName name="LOCAL_MYSQL_DATE_FORMAT" hidden="1">REPT(LOCAL_YEAR_FORMAT,4)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_MONTH_FORMAT,2)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_DAY_FORMAT,2)&amp;" "&amp;REPT(LOCAL_HOUR_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_MINUTE_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_SECOND_FORMAT,2)</definedName>
+  </definedNames>
   <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="305" uniqueCount="127">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="306" uniqueCount="127">
   <si>
     <t>id</t>
   </si>
@@ -210,9 +213,6 @@
     <t>nomor</t>
   </si>
   <si>
-    <t>tanggalItemStok</t>
-  </si>
-  <si>
     <t>tanggal</t>
   </si>
   <si>
@@ -412,6 +412,9 @@
   </si>
   <si>
     <t>modifiedBy</t>
+  </si>
+  <si>
+    <t>saldo</t>
   </si>
 </sst>
 </file>
@@ -1051,7 +1054,7 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B1" t="s">
         <v>17</v>
@@ -1060,7 +1063,7 @@
         <v>19</v>
       </c>
       <c r="D1" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
@@ -1188,10 +1191,10 @@
         <v>2</v>
       </c>
       <c r="D1" t="s">
+        <v>62</v>
+      </c>
+      <c r="E1" t="s">
         <v>63</v>
-      </c>
-      <c r="E1" t="s">
-        <v>64</v>
       </c>
       <c r="F1" t="s">
         <v>20</v>
@@ -1203,16 +1206,16 @@
         <v>58</v>
       </c>
       <c r="I1" t="s">
+        <v>59</v>
+      </c>
+      <c r="J1" t="s">
+        <v>64</v>
+      </c>
+      <c r="K1" t="s">
+        <v>81</v>
+      </c>
+      <c r="L1" t="s">
         <v>60</v>
-      </c>
-      <c r="J1" t="s">
-        <v>65</v>
-      </c>
-      <c r="K1" t="s">
-        <v>82</v>
-      </c>
-      <c r="L1" t="s">
-        <v>61</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.2">
@@ -1229,7 +1232,7 @@
         <v>1</v>
       </c>
       <c r="H2" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="I2" s="1">
         <v>41699</v>
@@ -1258,7 +1261,7 @@
         <v>2</v>
       </c>
       <c r="H3" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="I3" s="1">
         <v>41700</v>
@@ -1281,7 +1284,7 @@
         <v>6</v>
       </c>
       <c r="H4" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="I4" s="1">
         <v>41701</v>
@@ -1304,7 +1307,7 @@
         <v>6</v>
       </c>
       <c r="H5" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="I5" s="1">
         <v>41702</v>
@@ -1327,7 +1330,7 @@
         <v>6</v>
       </c>
       <c r="H6" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="I6" s="1">
         <v>41702</v>
@@ -1350,7 +1353,7 @@
         <v>6</v>
       </c>
       <c r="H7" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="I7" s="1">
         <v>41703</v>
@@ -1373,7 +1376,7 @@
         <v>6</v>
       </c>
       <c r="H8" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="I8" s="1">
         <v>41703</v>
@@ -1413,13 +1416,13 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B1" t="s">
+        <v>62</v>
+      </c>
+      <c r="C1" t="s">
         <v>63</v>
-      </c>
-      <c r="C1" t="s">
-        <v>64</v>
       </c>
       <c r="D1" t="s">
         <v>3</v>
@@ -1434,7 +1437,7 @@
         <v>19</v>
       </c>
       <c r="H1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
   </sheetData>
@@ -1445,10 +1448,10 @@
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L26"/>
+  <dimension ref="A1:M26"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M2" sqref="M2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1467,9 +1470,9 @@
     <col min="12" max="12" width="11" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B1" t="s">
         <v>17</v>
@@ -1481,31 +1484,34 @@
         <v>59</v>
       </c>
       <c r="E1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="F1" t="s">
+        <v>116</v>
+      </c>
+      <c r="G1" t="s">
         <v>117</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>118</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>119</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>120</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>121</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>122</v>
       </c>
-      <c r="L1" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M1" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>-1</v>
       </c>
@@ -1520,7 +1526,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>-2</v>
       </c>
@@ -1535,7 +1541,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>-3</v>
       </c>
@@ -1550,7 +1556,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>-4</v>
       </c>
@@ -1565,7 +1571,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>-5</v>
       </c>
@@ -1580,7 +1586,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>-6</v>
       </c>
@@ -1595,7 +1601,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>-6</v>
       </c>
@@ -1610,7 +1616,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>-7</v>
       </c>
@@ -1625,7 +1631,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>-8</v>
       </c>
@@ -1640,7 +1646,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>-9</v>
       </c>
@@ -1655,7 +1661,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>-10</v>
       </c>
@@ -1670,7 +1676,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>-11</v>
       </c>
@@ -1685,7 +1691,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>-12</v>
       </c>
@@ -1700,7 +1706,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>-12</v>
       </c>
@@ -1715,7 +1721,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>-13</v>
       </c>
@@ -1914,7 +1920,7 @@
         <v>58</v>
       </c>
       <c r="D1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E1" t="s">
         <v>1</v>
@@ -1929,7 +1935,7 @@
         <v>18</v>
       </c>
       <c r="I1" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
   </sheetData>
@@ -1954,7 +1960,7 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B1" t="s">
         <v>17</v>
@@ -1963,7 +1969,7 @@
         <v>19</v>
       </c>
       <c r="D1" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
   </sheetData>
@@ -2000,10 +2006,10 @@
         <v>0</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C1" s="5" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="D1" s="5" t="s">
         <v>1</v>
@@ -2015,7 +2021,7 @@
         <v>20</v>
       </c>
       <c r="G1" s="5" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="H1" s="5" t="s">
         <v>4</v>
@@ -2024,7 +2030,7 @@
         <v>58</v>
       </c>
       <c r="J1" s="5" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="K1" s="5" t="s">
         <v>18</v>
@@ -2040,7 +2046,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
@@ -2053,7 +2059,7 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" s="5" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B1" s="5" t="s">
         <v>3</v>
@@ -2065,7 +2071,7 @@
         <v>19</v>
       </c>
       <c r="E1" s="5" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
   </sheetData>
@@ -2094,7 +2100,7 @@
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
@@ -2109,13 +2115,13 @@
         <v>4</v>
       </c>
       <c r="F1" t="s">
+        <v>114</v>
+      </c>
+      <c r="G1" t="s">
         <v>115</v>
       </c>
-      <c r="G1" t="s">
-        <v>116</v>
-      </c>
       <c r="H1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="I1" t="s">
         <v>19</v>
@@ -2162,7 +2168,7 @@
         <v>5</v>
       </c>
       <c r="F1" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
@@ -2176,10 +2182,10 @@
         <v>6</v>
       </c>
       <c r="E2" t="s">
+        <v>97</v>
+      </c>
+      <c r="F2" t="s">
         <v>98</v>
-      </c>
-      <c r="F2" t="s">
-        <v>99</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
@@ -2193,10 +2199,10 @@
         <v>6</v>
       </c>
       <c r="E3" t="s">
+        <v>99</v>
+      </c>
+      <c r="F3" t="s">
         <v>100</v>
-      </c>
-      <c r="F3" t="s">
-        <v>101</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
@@ -2210,10 +2216,10 @@
         <v>6</v>
       </c>
       <c r="E4" t="s">
+        <v>101</v>
+      </c>
+      <c r="F4" t="s">
         <v>102</v>
-      </c>
-      <c r="F4" t="s">
-        <v>103</v>
       </c>
     </row>
   </sheetData>
@@ -2254,10 +2260,10 @@
         <v>2</v>
       </c>
       <c r="D1" t="s">
+        <v>105</v>
+      </c>
+      <c r="E1" t="s">
         <v>106</v>
-      </c>
-      <c r="E1" t="s">
-        <v>107</v>
       </c>
       <c r="F1" t="s">
         <v>4</v>
@@ -2269,25 +2275,25 @@
         <v>17</v>
       </c>
       <c r="I1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="J1" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="K1" t="s">
+        <v>111</v>
+      </c>
+      <c r="L1" t="s">
         <v>112</v>
       </c>
-      <c r="L1" t="s">
-        <v>113</v>
-      </c>
       <c r="M1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="N1" t="s">
         <v>20</v>
       </c>
       <c r="O1" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.2">
@@ -3197,10 +3203,10 @@
         <v>31</v>
       </c>
       <c r="I1" t="s">
+        <v>78</v>
+      </c>
+      <c r="J1" t="s">
         <v>79</v>
-      </c>
-      <c r="J1" t="s">
-        <v>80</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.2">
@@ -3851,10 +3857,10 @@
         <v>2</v>
       </c>
       <c r="D1" t="s">
+        <v>62</v>
+      </c>
+      <c r="E1" t="s">
         <v>63</v>
-      </c>
-      <c r="E1" t="s">
-        <v>64</v>
       </c>
       <c r="F1" t="s">
         <v>20</v>
@@ -3866,13 +3872,13 @@
         <v>58</v>
       </c>
       <c r="I1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="J1" t="s">
+        <v>89</v>
+      </c>
+      <c r="K1" t="s">
         <v>90</v>
-      </c>
-      <c r="K1" t="s">
-        <v>91</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.2">
@@ -3889,7 +3895,7 @@
         <v>1</v>
       </c>
       <c r="H2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="I2" s="3">
         <v>41699</v>
@@ -3915,7 +3921,7 @@
         <v>2</v>
       </c>
       <c r="H3" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="I3" s="1">
         <v>41700</v>
@@ -3935,7 +3941,7 @@
         <v>6</v>
       </c>
       <c r="H4" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="I4" s="1">
         <v>41701</v>
@@ -3955,7 +3961,7 @@
         <v>6</v>
       </c>
       <c r="H5" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="I5" s="1">
         <v>41702</v>
@@ -3975,7 +3981,7 @@
         <v>6</v>
       </c>
       <c r="H6" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="I6" s="1">
         <v>41702</v>
@@ -3995,7 +4001,7 @@
         <v>6</v>
       </c>
       <c r="H7" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="I7" s="1">
         <v>41703</v>
@@ -4015,7 +4021,7 @@
         <v>6</v>
       </c>
       <c r="H8" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="I8" s="1">
         <v>41703</v>
@@ -4052,13 +4058,13 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B1" t="s">
+        <v>62</v>
+      </c>
+      <c r="C1" t="s">
         <v>63</v>
-      </c>
-      <c r="C1" t="s">
-        <v>64</v>
       </c>
       <c r="D1" t="s">
         <v>3</v>
@@ -4073,7 +4079,7 @@
         <v>19</v>
       </c>
       <c r="H1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.2">
@@ -4291,16 +4297,16 @@
         <v>58</v>
       </c>
       <c r="G1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="H1" t="s">
         <v>18</v>
       </c>
       <c r="I1" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="J1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.2">
@@ -4314,7 +4320,7 @@
         <v>6</v>
       </c>
       <c r="F2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="G2" s="3">
         <v>41711</v>
@@ -4334,7 +4340,7 @@
         <v>6</v>
       </c>
       <c r="F3" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="G3" s="1">
         <v>41712</v>
@@ -4354,7 +4360,7 @@
         <v>6</v>
       </c>
       <c r="F4" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="G4" s="1">
         <v>41713</v>
@@ -4374,7 +4380,7 @@
         <v>6</v>
       </c>
       <c r="F5" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="G5" s="1">
         <v>41718</v>

</xml_diff>

<commit_message>
Change `NilaiPeriodik` from @Embeddable to entity.
</commit_message>
<xml_diff>
--- a/test/integration/project/data_inventory.xlsx
+++ b/test/integration/project/data_inventory.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="270" windowWidth="14940" windowHeight="7575" activeTab="2"/>
+    <workbookView xWindow="360" yWindow="270" windowWidth="14940" windowHeight="7575" firstSheet="9" activeTab="12"/>
   </bookViews>
   <sheets>
     <sheet name="Supplier" sheetId="6" r:id="rId1"/>
@@ -13,13 +13,13 @@
     <sheet name="Gudang" sheetId="1" r:id="rId4"/>
     <sheet name="StokProduk" sheetId="3" r:id="rId5"/>
     <sheet name="PeriodeItemStok" sheetId="5" r:id="rId6"/>
-    <sheet name="FakturBeli" sheetId="9" r:id="rId7"/>
-    <sheet name="FakturBeli_listItemFaktur" sheetId="10" r:id="rId8"/>
-    <sheet name="PenerimaanBarang" sheetId="7" r:id="rId9"/>
-    <sheet name="PenerimaanBarang_items" sheetId="8" r:id="rId10"/>
-    <sheet name="PurchaseOrder" sheetId="11" r:id="rId11"/>
-    <sheet name="PurchaseOrder_listItemFaktur" sheetId="12" r:id="rId12"/>
-    <sheet name="PeriodeItemStok_listItem" sheetId="4" r:id="rId13"/>
+    <sheet name="periodeitemstok_itemstok" sheetId="20" r:id="rId7"/>
+    <sheet name="FakturBeli" sheetId="9" r:id="rId8"/>
+    <sheet name="FakturBeli_listItemFaktur" sheetId="10" r:id="rId9"/>
+    <sheet name="PenerimaanBarang" sheetId="7" r:id="rId10"/>
+    <sheet name="PenerimaanBarang_items" sheetId="8" r:id="rId11"/>
+    <sheet name="PurchaseOrder" sheetId="11" r:id="rId12"/>
+    <sheet name="itemStok" sheetId="4" r:id="rId13"/>
     <sheet name="Transfer" sheetId="14" r:id="rId14"/>
     <sheet name="Transfer_items" sheetId="15" r:id="rId15"/>
     <sheet name="PenyesuaianStok" sheetId="16" r:id="rId16"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="307" uniqueCount="128">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="306" uniqueCount="128">
   <si>
     <t>id</t>
   </si>
@@ -321,9 +321,6 @@
     <t>PenerimaanBarang_id</t>
   </si>
   <si>
-    <t>PurchaseOrder_id</t>
-  </si>
-  <si>
     <t>singkatan</t>
   </si>
   <si>
@@ -418,6 +415,9 @@
   </si>
   <si>
     <t>ongkosKirimBeli</t>
+  </si>
+  <si>
+    <t>listItem_id</t>
   </si>
 </sst>
 </file>
@@ -1041,6 +1041,145 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:J5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H29" sqref="H29"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="2.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="6.140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="22" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="27.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>20</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>58</v>
+      </c>
+      <c r="G1" t="s">
+        <v>59</v>
+      </c>
+      <c r="H1" t="s">
+        <v>18</v>
+      </c>
+      <c r="I1" t="s">
+        <v>92</v>
+      </c>
+      <c r="J1" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A2">
+        <v>-1</v>
+      </c>
+      <c r="B2" s="3">
+        <v>41692</v>
+      </c>
+      <c r="C2" t="s">
+        <v>6</v>
+      </c>
+      <c r="F2" t="s">
+        <v>61</v>
+      </c>
+      <c r="G2" s="3">
+        <v>41711</v>
+      </c>
+      <c r="H2">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A3">
+        <v>-2</v>
+      </c>
+      <c r="B3" s="1">
+        <v>41692</v>
+      </c>
+      <c r="C3" t="s">
+        <v>6</v>
+      </c>
+      <c r="F3" t="s">
+        <v>66</v>
+      </c>
+      <c r="G3" s="1">
+        <v>41712</v>
+      </c>
+      <c r="H3">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A4">
+        <v>-3</v>
+      </c>
+      <c r="B4" s="1">
+        <v>41692</v>
+      </c>
+      <c r="C4" t="s">
+        <v>6</v>
+      </c>
+      <c r="F4" t="s">
+        <v>67</v>
+      </c>
+      <c r="G4" s="1">
+        <v>41713</v>
+      </c>
+      <c r="H4">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A5">
+        <v>-4</v>
+      </c>
+      <c r="B5" s="1">
+        <v>41353</v>
+      </c>
+      <c r="C5" t="s">
+        <v>6</v>
+      </c>
+      <c r="F5" t="s">
+        <v>69</v>
+      </c>
+      <c r="G5" s="1">
+        <v>41718</v>
+      </c>
+      <c r="H5">
+        <v>-1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1066,7 +1205,7 @@
         <v>19</v>
       </c>
       <c r="D1" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
@@ -1159,7 +1298,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L8"/>
   <sheetViews>
@@ -1397,85 +1536,34 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H1"/>
+  <dimension ref="A1:Q26"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="N2" sqref="N2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="16" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="5.5703125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="6.42578125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="20.140625" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
-        <v>95</v>
-      </c>
-      <c r="B1" t="s">
-        <v>62</v>
-      </c>
-      <c r="C1" t="s">
-        <v>63</v>
-      </c>
-      <c r="D1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" t="s">
-        <v>17</v>
-      </c>
-      <c r="F1" t="s">
-        <v>20</v>
-      </c>
-      <c r="G1" t="s">
-        <v>19</v>
-      </c>
-      <c r="H1" t="s">
-        <v>76</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M26"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="M2" sqref="M2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="17.42578125" customWidth="1"/>
     <col min="2" max="2" width="10.140625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="20.28515625" style="1" customWidth="1"/>
     <col min="4" max="4" width="19.7109375" customWidth="1"/>
-    <col min="5" max="5" width="17.42578125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11.85546875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="9.85546875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="10.28515625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="12.5703125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="11" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="11" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="11" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="10.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>68</v>
+        <v>0</v>
       </c>
       <c r="B1" t="s">
         <v>17</v>
@@ -1487,7 +1575,7 @@
         <v>59</v>
       </c>
       <c r="E1" t="s">
-        <v>80</v>
+        <v>115</v>
       </c>
       <c r="F1" t="s">
         <v>116</v>
@@ -1508,13 +1596,25 @@
         <v>121</v>
       </c>
       <c r="L1" t="s">
-        <v>122</v>
+        <v>125</v>
       </c>
       <c r="M1" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+      <c r="N1" t="s">
+        <v>123</v>
+      </c>
+      <c r="O1" t="s">
+        <v>2</v>
+      </c>
+      <c r="P1" t="s">
+        <v>4</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="2" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>-1</v>
       </c>
@@ -1525,11 +1625,8 @@
       <c r="D2" s="3">
         <v>41628</v>
       </c>
-      <c r="E2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
+    </row>
+    <row r="3" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>-2</v>
       </c>
@@ -1540,11 +1637,8 @@
       <c r="D3" s="3">
         <v>41654</v>
       </c>
-      <c r="E3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
+    </row>
+    <row r="4" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>-3</v>
       </c>
@@ -1555,11 +1649,8 @@
       <c r="D4" s="3">
         <v>41649</v>
       </c>
-      <c r="E4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
+    </row>
+    <row r="5" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>-4</v>
       </c>
@@ -1570,11 +1661,8 @@
       <c r="D5" s="3">
         <v>41678</v>
       </c>
-      <c r="E5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.2">
+    </row>
+    <row r="6" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>-5</v>
       </c>
@@ -1585,11 +1673,8 @@
       <c r="D6" s="3">
         <v>41654</v>
       </c>
-      <c r="E6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.2">
+    </row>
+    <row r="7" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>-6</v>
       </c>
@@ -1600,13 +1685,10 @@
       <c r="D7" s="3">
         <v>41649</v>
       </c>
-      <c r="E7">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.2">
+    </row>
+    <row r="8" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A8">
-        <v>-6</v>
+        <v>-7</v>
       </c>
       <c r="B8">
         <v>2</v>
@@ -1615,13 +1697,10 @@
       <c r="D8" s="3">
         <v>41651</v>
       </c>
-      <c r="E8">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.2">
+    </row>
+    <row r="9" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A9">
-        <v>-7</v>
+        <v>-8</v>
       </c>
       <c r="B9">
         <v>3</v>
@@ -1630,13 +1709,10 @@
       <c r="D9" s="3">
         <v>41654</v>
       </c>
-      <c r="E9">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.2">
+    </row>
+    <row r="10" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A10">
-        <v>-8</v>
+        <v>-9</v>
       </c>
       <c r="B10">
         <v>2</v>
@@ -1645,13 +1721,10 @@
       <c r="D10" s="3">
         <v>41654</v>
       </c>
-      <c r="E10">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.2">
+    </row>
+    <row r="11" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A11">
-        <v>-9</v>
+        <v>-10</v>
       </c>
       <c r="B11">
         <v>3</v>
@@ -1660,13 +1733,10 @@
       <c r="D11" s="3">
         <v>41654</v>
       </c>
-      <c r="E11">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.2">
+    </row>
+    <row r="12" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A12">
-        <v>-10</v>
+        <v>-11</v>
       </c>
       <c r="B12">
         <v>2</v>
@@ -1675,13 +1745,10 @@
       <c r="D12" s="3">
         <v>41640</v>
       </c>
-      <c r="E12">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.2">
+    </row>
+    <row r="13" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A13">
-        <v>-11</v>
+        <v>-12</v>
       </c>
       <c r="B13">
         <v>2</v>
@@ -1690,13 +1757,10 @@
       <c r="D13" s="3">
         <v>41672</v>
       </c>
-      <c r="E13">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.2">
+    </row>
+    <row r="14" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A14">
-        <v>-12</v>
+        <v>-13</v>
       </c>
       <c r="B14">
         <v>3</v>
@@ -1705,13 +1769,10 @@
       <c r="D14" s="3">
         <v>41640</v>
       </c>
-      <c r="E14">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.2">
+    </row>
+    <row r="15" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A15">
-        <v>-12</v>
+        <v>-14</v>
       </c>
       <c r="B15">
         <v>2</v>
@@ -1720,13 +1781,10 @@
       <c r="D15" s="3">
         <v>41669</v>
       </c>
-      <c r="E15">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.2">
+    </row>
+    <row r="16" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A16">
-        <v>-13</v>
+        <v>-15</v>
       </c>
       <c r="B16">
         <v>1</v>
@@ -1735,13 +1793,10 @@
       <c r="D16" s="3">
         <v>41672</v>
       </c>
-      <c r="E16">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A17">
-        <v>-14</v>
+        <v>-16</v>
       </c>
       <c r="B17">
         <v>7</v>
@@ -1750,13 +1805,10 @@
       <c r="D17" s="3">
         <v>41685</v>
       </c>
-      <c r="E17">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A18">
-        <v>-15</v>
+        <v>-17</v>
       </c>
       <c r="B18">
         <v>8</v>
@@ -1765,13 +1817,10 @@
       <c r="D18" s="3">
         <v>41685</v>
       </c>
-      <c r="E18">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A19">
-        <v>-16</v>
+        <v>-18</v>
       </c>
       <c r="B19">
         <v>9</v>
@@ -1780,13 +1829,10 @@
       <c r="D19" s="3">
         <v>41692</v>
       </c>
-      <c r="E19">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A20">
-        <v>-17</v>
+        <v>-19</v>
       </c>
       <c r="B20">
         <v>4</v>
@@ -1795,13 +1841,10 @@
       <c r="D20" s="3">
         <v>41646</v>
       </c>
-      <c r="E20">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A21">
-        <v>-18</v>
+        <v>-20</v>
       </c>
       <c r="B21">
         <v>3</v>
@@ -1810,13 +1853,10 @@
       <c r="D21" s="1">
         <v>40179</v>
       </c>
-      <c r="E21">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A22">
-        <v>-18</v>
+        <v>-21</v>
       </c>
       <c r="B22">
         <v>5</v>
@@ -1825,13 +1865,10 @@
       <c r="D22" s="1">
         <v>40188</v>
       </c>
-      <c r="E22">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A23">
-        <v>-18</v>
+        <v>-22</v>
       </c>
       <c r="B23">
         <v>2</v>
@@ -1840,13 +1877,10 @@
       <c r="D23" s="1">
         <v>40198</v>
       </c>
-      <c r="E23">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A24">
-        <v>-19</v>
+        <v>-23</v>
       </c>
       <c r="B24">
         <v>5</v>
@@ -1854,13 +1888,10 @@
       <c r="D24" s="1">
         <v>41353</v>
       </c>
-      <c r="E24">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A25">
-        <v>-20</v>
+        <v>-24</v>
       </c>
       <c r="B25">
         <v>10</v>
@@ -1868,22 +1899,16 @@
       <c r="D25" s="1">
         <v>41353</v>
       </c>
-      <c r="E25">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A26">
-        <v>-21</v>
+        <v>-25</v>
       </c>
       <c r="B26">
         <v>7</v>
       </c>
       <c r="D26" s="1">
         <v>41353</v>
-      </c>
-      <c r="E26">
-        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -1938,7 +1963,7 @@
         <v>18</v>
       </c>
       <c r="I1" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
   </sheetData>
@@ -1963,7 +1988,7 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B1" t="s">
         <v>17</v>
@@ -1972,7 +1997,7 @@
         <v>19</v>
       </c>
       <c r="D1" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
   </sheetData>
@@ -2009,10 +2034,10 @@
         <v>0</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C1" s="5" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="D1" s="5" t="s">
         <v>1</v>
@@ -2024,7 +2049,7 @@
         <v>20</v>
       </c>
       <c r="G1" s="5" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="H1" s="5" t="s">
         <v>4</v>
@@ -2062,7 +2087,7 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" s="5" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B1" s="5" t="s">
         <v>3</v>
@@ -2074,7 +2099,7 @@
         <v>19</v>
       </c>
       <c r="E1" s="5" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
   </sheetData>
@@ -2103,7 +2128,7 @@
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
@@ -2118,10 +2143,10 @@
         <v>4</v>
       </c>
       <c r="F1" t="s">
+        <v>113</v>
+      </c>
+      <c r="G1" t="s">
         <v>114</v>
-      </c>
-      <c r="G1" t="s">
-        <v>115</v>
       </c>
       <c r="H1" t="s">
         <v>59</v>
@@ -2171,7 +2196,7 @@
         <v>5</v>
       </c>
       <c r="F1" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
@@ -2185,10 +2210,10 @@
         <v>6</v>
       </c>
       <c r="E2" t="s">
+        <v>96</v>
+      </c>
+      <c r="F2" t="s">
         <v>97</v>
-      </c>
-      <c r="F2" t="s">
-        <v>98</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
@@ -2202,10 +2227,10 @@
         <v>6</v>
       </c>
       <c r="E3" t="s">
+        <v>98</v>
+      </c>
+      <c r="F3" t="s">
         <v>99</v>
-      </c>
-      <c r="F3" t="s">
-        <v>100</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
@@ -2219,10 +2244,10 @@
         <v>6</v>
       </c>
       <c r="E4" t="s">
+        <v>100</v>
+      </c>
+      <c r="F4" t="s">
         <v>101</v>
-      </c>
-      <c r="F4" t="s">
-        <v>102</v>
       </c>
     </row>
   </sheetData>
@@ -2235,7 +2260,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
@@ -2263,13 +2288,13 @@
         <v>2</v>
       </c>
       <c r="D1" t="s">
+        <v>104</v>
+      </c>
+      <c r="E1" t="s">
         <v>105</v>
       </c>
-      <c r="E1" t="s">
-        <v>106</v>
-      </c>
       <c r="F1" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="G1" t="s">
         <v>4</v>
@@ -2284,13 +2309,13 @@
         <v>77</v>
       </c>
       <c r="K1" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="L1" t="s">
+        <v>110</v>
+      </c>
+      <c r="M1" t="s">
         <v>111</v>
-      </c>
-      <c r="M1" t="s">
-        <v>112</v>
       </c>
       <c r="N1" t="s">
         <v>60</v>
@@ -2299,7 +2324,7 @@
         <v>20</v>
       </c>
       <c r="P1" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.2">
@@ -3832,6 +3857,312 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C26"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2:B26"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="17.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>68</v>
+      </c>
+      <c r="B1" t="s">
+        <v>127</v>
+      </c>
+      <c r="C1" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2">
+        <v>-1</v>
+      </c>
+      <c r="B2">
+        <v>-1</v>
+      </c>
+      <c r="C2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A3">
+        <v>-2</v>
+      </c>
+      <c r="B3">
+        <v>-2</v>
+      </c>
+      <c r="C3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A4">
+        <v>-3</v>
+      </c>
+      <c r="B4">
+        <v>-3</v>
+      </c>
+      <c r="C4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A5">
+        <v>-4</v>
+      </c>
+      <c r="B5">
+        <v>-4</v>
+      </c>
+      <c r="C5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A6">
+        <v>-5</v>
+      </c>
+      <c r="B6">
+        <v>-5</v>
+      </c>
+      <c r="C6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A7">
+        <v>-6</v>
+      </c>
+      <c r="B7">
+        <v>-6</v>
+      </c>
+      <c r="C7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A8">
+        <v>-6</v>
+      </c>
+      <c r="B8">
+        <v>-7</v>
+      </c>
+      <c r="C8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A9">
+        <v>-7</v>
+      </c>
+      <c r="B9">
+        <v>-8</v>
+      </c>
+      <c r="C9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A10">
+        <v>-8</v>
+      </c>
+      <c r="B10">
+        <v>-9</v>
+      </c>
+      <c r="C10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A11">
+        <v>-9</v>
+      </c>
+      <c r="B11">
+        <v>-10</v>
+      </c>
+      <c r="C11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A12">
+        <v>-10</v>
+      </c>
+      <c r="B12">
+        <v>-11</v>
+      </c>
+      <c r="C12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A13">
+        <v>-11</v>
+      </c>
+      <c r="B13">
+        <v>-12</v>
+      </c>
+      <c r="C13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A14">
+        <v>-12</v>
+      </c>
+      <c r="B14">
+        <v>-13</v>
+      </c>
+      <c r="C14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A15">
+        <v>-12</v>
+      </c>
+      <c r="B15">
+        <v>-14</v>
+      </c>
+      <c r="C15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A16">
+        <v>-13</v>
+      </c>
+      <c r="B16">
+        <v>-15</v>
+      </c>
+      <c r="C16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A17">
+        <v>-14</v>
+      </c>
+      <c r="B17">
+        <v>-16</v>
+      </c>
+      <c r="C17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A18">
+        <v>-15</v>
+      </c>
+      <c r="B18">
+        <v>-17</v>
+      </c>
+      <c r="C18">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A19">
+        <v>-16</v>
+      </c>
+      <c r="B19">
+        <v>-18</v>
+      </c>
+      <c r="C19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A20">
+        <v>-17</v>
+      </c>
+      <c r="B20">
+        <v>-19</v>
+      </c>
+      <c r="C20">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A21">
+        <v>-18</v>
+      </c>
+      <c r="B21">
+        <v>-20</v>
+      </c>
+      <c r="C21">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A22">
+        <v>-18</v>
+      </c>
+      <c r="B22">
+        <v>-21</v>
+      </c>
+      <c r="C22">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A23">
+        <v>-18</v>
+      </c>
+      <c r="B23">
+        <v>-22</v>
+      </c>
+      <c r="C23">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A24">
+        <v>-19</v>
+      </c>
+      <c r="B24">
+        <v>-23</v>
+      </c>
+      <c r="C24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A25">
+        <v>-20</v>
+      </c>
+      <c r="B25">
+        <v>-24</v>
+      </c>
+      <c r="C25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A26">
+        <v>-21</v>
+      </c>
+      <c r="B26">
+        <v>-25</v>
+      </c>
+      <c r="C26">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -4042,7 +4373,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H10"/>
   <sheetViews>
@@ -4260,143 +4591,4 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J5"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H29" sqref="H29"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="2.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="7" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="6.140625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="22" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="27.28515625" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" t="s">
-        <v>20</v>
-      </c>
-      <c r="E1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" t="s">
-        <v>58</v>
-      </c>
-      <c r="G1" t="s">
-        <v>59</v>
-      </c>
-      <c r="H1" t="s">
-        <v>18</v>
-      </c>
-      <c r="I1" t="s">
-        <v>92</v>
-      </c>
-      <c r="J1" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A2">
-        <v>-1</v>
-      </c>
-      <c r="B2" s="3">
-        <v>41692</v>
-      </c>
-      <c r="C2" t="s">
-        <v>6</v>
-      </c>
-      <c r="F2" t="s">
-        <v>61</v>
-      </c>
-      <c r="G2" s="3">
-        <v>41711</v>
-      </c>
-      <c r="H2">
-        <v>-1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A3">
-        <v>-2</v>
-      </c>
-      <c r="B3" s="1">
-        <v>41692</v>
-      </c>
-      <c r="C3" t="s">
-        <v>6</v>
-      </c>
-      <c r="F3" t="s">
-        <v>66</v>
-      </c>
-      <c r="G3" s="1">
-        <v>41712</v>
-      </c>
-      <c r="H3">
-        <v>-1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A4">
-        <v>-3</v>
-      </c>
-      <c r="B4" s="1">
-        <v>41692</v>
-      </c>
-      <c r="C4" t="s">
-        <v>6</v>
-      </c>
-      <c r="F4" t="s">
-        <v>67</v>
-      </c>
-      <c r="G4" s="1">
-        <v>41713</v>
-      </c>
-      <c r="H4">
-        <v>-1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A5">
-        <v>-4</v>
-      </c>
-      <c r="B5" s="1">
-        <v>41353</v>
-      </c>
-      <c r="C5" t="s">
-        <v>6</v>
-      </c>
-      <c r="F5" t="s">
-        <v>69</v>
-      </c>
-      <c r="G5" s="1">
-        <v>41718</v>
-      </c>
-      <c r="H5">
-        <v>-1</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
Tuning queries income statements to increase speed.
</commit_message>
<xml_diff>
--- a/test/integration/project/data_inventory.xlsx
+++ b/test/integration/project/data_inventory.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="270" windowWidth="14940" windowHeight="7575" firstSheet="9" activeTab="12"/>
+    <workbookView xWindow="360" yWindow="270" windowWidth="14940" windowHeight="7575" firstSheet="3" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="Supplier" sheetId="6" r:id="rId1"/>
@@ -14,12 +14,12 @@
     <sheet name="StokProduk" sheetId="3" r:id="rId5"/>
     <sheet name="PeriodeItemStok" sheetId="5" r:id="rId6"/>
     <sheet name="periodeitemstok_itemstok" sheetId="20" r:id="rId7"/>
-    <sheet name="FakturBeli" sheetId="9" r:id="rId8"/>
-    <sheet name="FakturBeli_listItemFaktur" sheetId="10" r:id="rId9"/>
-    <sheet name="PenerimaanBarang" sheetId="7" r:id="rId10"/>
-    <sheet name="PenerimaanBarang_items" sheetId="8" r:id="rId11"/>
-    <sheet name="PurchaseOrder" sheetId="11" r:id="rId12"/>
-    <sheet name="itemStok" sheetId="4" r:id="rId13"/>
+    <sheet name="itemStok" sheetId="4" r:id="rId8"/>
+    <sheet name="FakturBeli" sheetId="9" r:id="rId9"/>
+    <sheet name="FakturBeli_listItemFaktur" sheetId="10" r:id="rId10"/>
+    <sheet name="PenerimaanBarang" sheetId="7" r:id="rId11"/>
+    <sheet name="PenerimaanBarang_items" sheetId="8" r:id="rId12"/>
+    <sheet name="PurchaseOrder" sheetId="11" r:id="rId13"/>
     <sheet name="Transfer" sheetId="14" r:id="rId14"/>
     <sheet name="Transfer_items" sheetId="15" r:id="rId15"/>
     <sheet name="PenyesuaianStok" sheetId="16" r:id="rId16"/>
@@ -1041,6 +1041,226 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:H10"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="5.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="6.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="20.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>93</v>
+      </c>
+      <c r="B1" t="s">
+        <v>62</v>
+      </c>
+      <c r="C1" t="s">
+        <v>63</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>17</v>
+      </c>
+      <c r="F1" t="s">
+        <v>20</v>
+      </c>
+      <c r="G1" t="s">
+        <v>19</v>
+      </c>
+      <c r="H1" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A2">
+        <v>-1</v>
+      </c>
+      <c r="B2">
+        <v>100</v>
+      </c>
+      <c r="C2">
+        <v>1</v>
+      </c>
+      <c r="D2">
+        <v>1000</v>
+      </c>
+      <c r="E2">
+        <v>5</v>
+      </c>
+      <c r="G2">
+        <v>-1</v>
+      </c>
+      <c r="H2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A3">
+        <v>-1</v>
+      </c>
+      <c r="C3">
+        <v>2</v>
+      </c>
+      <c r="D3">
+        <v>2000</v>
+      </c>
+      <c r="E3">
+        <v>3</v>
+      </c>
+      <c r="G3">
+        <v>-2</v>
+      </c>
+      <c r="H3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A4">
+        <v>-1</v>
+      </c>
+      <c r="C4">
+        <v>3</v>
+      </c>
+      <c r="D4">
+        <v>3000</v>
+      </c>
+      <c r="E4">
+        <v>4</v>
+      </c>
+      <c r="G4">
+        <v>-3</v>
+      </c>
+      <c r="H4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A5">
+        <v>-2</v>
+      </c>
+      <c r="C5">
+        <v>4</v>
+      </c>
+      <c r="D5">
+        <v>1500</v>
+      </c>
+      <c r="E5">
+        <v>2</v>
+      </c>
+      <c r="G5">
+        <v>-1</v>
+      </c>
+      <c r="H5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A6">
+        <v>-3</v>
+      </c>
+      <c r="D6">
+        <v>1400</v>
+      </c>
+      <c r="E6">
+        <v>1</v>
+      </c>
+      <c r="G6">
+        <v>-2</v>
+      </c>
+      <c r="H6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A7">
+        <v>-4</v>
+      </c>
+      <c r="D7">
+        <v>2000</v>
+      </c>
+      <c r="E7">
+        <v>1</v>
+      </c>
+      <c r="G7">
+        <v>-3</v>
+      </c>
+      <c r="H7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A8">
+        <v>-5</v>
+      </c>
+      <c r="D8">
+        <v>1900</v>
+      </c>
+      <c r="E8">
+        <v>2</v>
+      </c>
+      <c r="G8">
+        <v>-1</v>
+      </c>
+      <c r="H8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A9">
+        <v>-6</v>
+      </c>
+      <c r="D9">
+        <v>1700</v>
+      </c>
+      <c r="E9">
+        <v>1</v>
+      </c>
+      <c r="G9">
+        <v>-1</v>
+      </c>
+      <c r="H9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A10">
+        <v>-7</v>
+      </c>
+      <c r="D10">
+        <v>1800</v>
+      </c>
+      <c r="E10">
+        <v>1</v>
+      </c>
+      <c r="G10">
+        <v>-1</v>
+      </c>
+      <c r="H10">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1178,7 +1398,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D7"/>
   <sheetViews>
@@ -1298,7 +1518,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L8"/>
   <sheetViews>
@@ -1533,388 +1753,6 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q26"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N2" sqref="N2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="2" max="2" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="20.28515625" style="1" customWidth="1"/>
-    <col min="4" max="4" width="19.7109375" customWidth="1"/>
-    <col min="5" max="5" width="12" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.85546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9.85546875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.28515625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="12.5703125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="11" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="11" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="11.7109375" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="10.140625" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>17</v>
-      </c>
-      <c r="C1" t="s">
-        <v>20</v>
-      </c>
-      <c r="D1" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="E1" t="s">
-        <v>115</v>
-      </c>
-      <c r="F1" t="s">
-        <v>116</v>
-      </c>
-      <c r="G1" t="s">
-        <v>117</v>
-      </c>
-      <c r="H1" t="s">
-        <v>118</v>
-      </c>
-      <c r="I1" t="s">
-        <v>119</v>
-      </c>
-      <c r="J1" t="s">
-        <v>120</v>
-      </c>
-      <c r="K1" t="s">
-        <v>121</v>
-      </c>
-      <c r="L1" t="s">
-        <v>125</v>
-      </c>
-      <c r="M1" t="s">
-        <v>1</v>
-      </c>
-      <c r="N1" t="s">
-        <v>123</v>
-      </c>
-      <c r="O1" t="s">
-        <v>2</v>
-      </c>
-      <c r="P1" t="s">
-        <v>4</v>
-      </c>
-      <c r="Q1" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A2">
-        <v>-1</v>
-      </c>
-      <c r="B2">
-        <v>3</v>
-      </c>
-      <c r="C2"/>
-      <c r="D2" s="3">
-        <v>41628</v>
-      </c>
-    </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A3">
-        <v>-2</v>
-      </c>
-      <c r="B3">
-        <v>2</v>
-      </c>
-      <c r="C3"/>
-      <c r="D3" s="3">
-        <v>41654</v>
-      </c>
-    </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A4">
-        <v>-3</v>
-      </c>
-      <c r="B4">
-        <v>2</v>
-      </c>
-      <c r="C4"/>
-      <c r="D4" s="3">
-        <v>41649</v>
-      </c>
-    </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A5">
-        <v>-4</v>
-      </c>
-      <c r="B5">
-        <v>2</v>
-      </c>
-      <c r="C5"/>
-      <c r="D5" s="3">
-        <v>41678</v>
-      </c>
-    </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A6">
-        <v>-5</v>
-      </c>
-      <c r="B6">
-        <v>10</v>
-      </c>
-      <c r="C6"/>
-      <c r="D6" s="3">
-        <v>41654</v>
-      </c>
-    </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A7">
-        <v>-6</v>
-      </c>
-      <c r="B7">
-        <v>3</v>
-      </c>
-      <c r="C7"/>
-      <c r="D7" s="3">
-        <v>41649</v>
-      </c>
-    </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A8">
-        <v>-7</v>
-      </c>
-      <c r="B8">
-        <v>2</v>
-      </c>
-      <c r="C8"/>
-      <c r="D8" s="3">
-        <v>41651</v>
-      </c>
-    </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A9">
-        <v>-8</v>
-      </c>
-      <c r="B9">
-        <v>3</v>
-      </c>
-      <c r="C9"/>
-      <c r="D9" s="3">
-        <v>41654</v>
-      </c>
-    </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A10">
-        <v>-9</v>
-      </c>
-      <c r="B10">
-        <v>2</v>
-      </c>
-      <c r="C10"/>
-      <c r="D10" s="3">
-        <v>41654</v>
-      </c>
-    </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A11">
-        <v>-10</v>
-      </c>
-      <c r="B11">
-        <v>3</v>
-      </c>
-      <c r="C11"/>
-      <c r="D11" s="3">
-        <v>41654</v>
-      </c>
-    </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A12">
-        <v>-11</v>
-      </c>
-      <c r="B12">
-        <v>2</v>
-      </c>
-      <c r="C12"/>
-      <c r="D12" s="3">
-        <v>41640</v>
-      </c>
-    </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A13">
-        <v>-12</v>
-      </c>
-      <c r="B13">
-        <v>2</v>
-      </c>
-      <c r="C13"/>
-      <c r="D13" s="3">
-        <v>41672</v>
-      </c>
-    </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A14">
-        <v>-13</v>
-      </c>
-      <c r="B14">
-        <v>3</v>
-      </c>
-      <c r="C14"/>
-      <c r="D14" s="3">
-        <v>41640</v>
-      </c>
-    </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A15">
-        <v>-14</v>
-      </c>
-      <c r="B15">
-        <v>2</v>
-      </c>
-      <c r="C15"/>
-      <c r="D15" s="3">
-        <v>41669</v>
-      </c>
-    </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A16">
-        <v>-15</v>
-      </c>
-      <c r="B16">
-        <v>1</v>
-      </c>
-      <c r="C16"/>
-      <c r="D16" s="3">
-        <v>41672</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A17">
-        <v>-16</v>
-      </c>
-      <c r="B17">
-        <v>7</v>
-      </c>
-      <c r="C17"/>
-      <c r="D17" s="3">
-        <v>41685</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A18">
-        <v>-17</v>
-      </c>
-      <c r="B18">
-        <v>8</v>
-      </c>
-      <c r="C18"/>
-      <c r="D18" s="3">
-        <v>41685</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A19">
-        <v>-18</v>
-      </c>
-      <c r="B19">
-        <v>9</v>
-      </c>
-      <c r="C19"/>
-      <c r="D19" s="3">
-        <v>41692</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A20">
-        <v>-19</v>
-      </c>
-      <c r="B20">
-        <v>4</v>
-      </c>
-      <c r="C20"/>
-      <c r="D20" s="3">
-        <v>41646</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A21">
-        <v>-20</v>
-      </c>
-      <c r="B21">
-        <v>3</v>
-      </c>
-      <c r="C21"/>
-      <c r="D21" s="1">
-        <v>40179</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A22">
-        <v>-21</v>
-      </c>
-      <c r="B22">
-        <v>5</v>
-      </c>
-      <c r="C22"/>
-      <c r="D22" s="1">
-        <v>40188</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A23">
-        <v>-22</v>
-      </c>
-      <c r="B23">
-        <v>2</v>
-      </c>
-      <c r="C23"/>
-      <c r="D23" s="1">
-        <v>40198</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A24">
-        <v>-23</v>
-      </c>
-      <c r="B24">
-        <v>5</v>
-      </c>
-      <c r="D24" s="1">
-        <v>41353</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A25">
-        <v>-24</v>
-      </c>
-      <c r="B25">
-        <v>10</v>
-      </c>
-      <c r="D25" s="1">
-        <v>41353</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A26">
-        <v>-25</v>
-      </c>
-      <c r="B26">
-        <v>7</v>
-      </c>
-      <c r="D26" s="1">
-        <v>41353</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" copies="0"/>
-  <headerFooter alignWithMargins="0"/>
 </worksheet>
 </file>
 
@@ -2862,7 +2700,7 @@
   <dimension ref="A1:G15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D2" sqref="D2:D8"/>
+      <selection activeCell="H30" sqref="H30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -3191,7 +3029,7 @@
   <dimension ref="A1:J22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J1" sqref="I1:J1"/>
+      <selection activeCell="A22" sqref="A22:J22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -4163,6 +4001,388 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:Q26"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="N2" sqref="N2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="20.28515625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="19.7109375" customWidth="1"/>
+    <col min="5" max="5" width="12" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="11" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="11" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="10.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="E1" t="s">
+        <v>115</v>
+      </c>
+      <c r="F1" t="s">
+        <v>116</v>
+      </c>
+      <c r="G1" t="s">
+        <v>117</v>
+      </c>
+      <c r="H1" t="s">
+        <v>118</v>
+      </c>
+      <c r="I1" t="s">
+        <v>119</v>
+      </c>
+      <c r="J1" t="s">
+        <v>120</v>
+      </c>
+      <c r="K1" t="s">
+        <v>121</v>
+      </c>
+      <c r="L1" t="s">
+        <v>125</v>
+      </c>
+      <c r="M1" t="s">
+        <v>1</v>
+      </c>
+      <c r="N1" t="s">
+        <v>123</v>
+      </c>
+      <c r="O1" t="s">
+        <v>2</v>
+      </c>
+      <c r="P1" t="s">
+        <v>4</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="2" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A2">
+        <v>-1</v>
+      </c>
+      <c r="B2">
+        <v>3</v>
+      </c>
+      <c r="C2"/>
+      <c r="D2" s="3">
+        <v>41628</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A3">
+        <v>-2</v>
+      </c>
+      <c r="B3">
+        <v>2</v>
+      </c>
+      <c r="C3"/>
+      <c r="D3" s="3">
+        <v>41654</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A4">
+        <v>-3</v>
+      </c>
+      <c r="B4">
+        <v>2</v>
+      </c>
+      <c r="C4"/>
+      <c r="D4" s="3">
+        <v>41649</v>
+      </c>
+    </row>
+    <row r="5" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A5">
+        <v>-4</v>
+      </c>
+      <c r="B5">
+        <v>2</v>
+      </c>
+      <c r="C5"/>
+      <c r="D5" s="3">
+        <v>41678</v>
+      </c>
+    </row>
+    <row r="6" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A6">
+        <v>-5</v>
+      </c>
+      <c r="B6">
+        <v>10</v>
+      </c>
+      <c r="C6"/>
+      <c r="D6" s="3">
+        <v>41654</v>
+      </c>
+    </row>
+    <row r="7" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A7">
+        <v>-6</v>
+      </c>
+      <c r="B7">
+        <v>3</v>
+      </c>
+      <c r="C7"/>
+      <c r="D7" s="3">
+        <v>41649</v>
+      </c>
+    </row>
+    <row r="8" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A8">
+        <v>-7</v>
+      </c>
+      <c r="B8">
+        <v>2</v>
+      </c>
+      <c r="C8"/>
+      <c r="D8" s="3">
+        <v>41651</v>
+      </c>
+    </row>
+    <row r="9" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A9">
+        <v>-8</v>
+      </c>
+      <c r="B9">
+        <v>3</v>
+      </c>
+      <c r="C9"/>
+      <c r="D9" s="3">
+        <v>41654</v>
+      </c>
+    </row>
+    <row r="10" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A10">
+        <v>-9</v>
+      </c>
+      <c r="B10">
+        <v>2</v>
+      </c>
+      <c r="C10"/>
+      <c r="D10" s="3">
+        <v>41654</v>
+      </c>
+    </row>
+    <row r="11" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A11">
+        <v>-10</v>
+      </c>
+      <c r="B11">
+        <v>3</v>
+      </c>
+      <c r="C11"/>
+      <c r="D11" s="3">
+        <v>41654</v>
+      </c>
+    </row>
+    <row r="12" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A12">
+        <v>-11</v>
+      </c>
+      <c r="B12">
+        <v>2</v>
+      </c>
+      <c r="C12"/>
+      <c r="D12" s="3">
+        <v>41640</v>
+      </c>
+    </row>
+    <row r="13" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A13">
+        <v>-12</v>
+      </c>
+      <c r="B13">
+        <v>2</v>
+      </c>
+      <c r="C13"/>
+      <c r="D13" s="3">
+        <v>41672</v>
+      </c>
+    </row>
+    <row r="14" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A14">
+        <v>-13</v>
+      </c>
+      <c r="B14">
+        <v>3</v>
+      </c>
+      <c r="C14"/>
+      <c r="D14" s="3">
+        <v>41640</v>
+      </c>
+    </row>
+    <row r="15" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A15">
+        <v>-14</v>
+      </c>
+      <c r="B15">
+        <v>2</v>
+      </c>
+      <c r="C15"/>
+      <c r="D15" s="3">
+        <v>41669</v>
+      </c>
+    </row>
+    <row r="16" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A16">
+        <v>-15</v>
+      </c>
+      <c r="B16">
+        <v>1</v>
+      </c>
+      <c r="C16"/>
+      <c r="D16" s="3">
+        <v>41672</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A17">
+        <v>-16</v>
+      </c>
+      <c r="B17">
+        <v>7</v>
+      </c>
+      <c r="C17"/>
+      <c r="D17" s="3">
+        <v>41685</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A18">
+        <v>-17</v>
+      </c>
+      <c r="B18">
+        <v>8</v>
+      </c>
+      <c r="C18"/>
+      <c r="D18" s="3">
+        <v>41685</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A19">
+        <v>-18</v>
+      </c>
+      <c r="B19">
+        <v>9</v>
+      </c>
+      <c r="C19"/>
+      <c r="D19" s="3">
+        <v>41692</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A20">
+        <v>-19</v>
+      </c>
+      <c r="B20">
+        <v>4</v>
+      </c>
+      <c r="C20"/>
+      <c r="D20" s="3">
+        <v>41646</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A21">
+        <v>-20</v>
+      </c>
+      <c r="B21">
+        <v>3</v>
+      </c>
+      <c r="C21"/>
+      <c r="D21" s="1">
+        <v>40179</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A22">
+        <v>-21</v>
+      </c>
+      <c r="B22">
+        <v>5</v>
+      </c>
+      <c r="C22"/>
+      <c r="D22" s="1">
+        <v>40188</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A23">
+        <v>-22</v>
+      </c>
+      <c r="B23">
+        <v>2</v>
+      </c>
+      <c r="C23"/>
+      <c r="D23" s="1">
+        <v>40198</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A24">
+        <v>-23</v>
+      </c>
+      <c r="B24">
+        <v>5</v>
+      </c>
+      <c r="D24" s="1">
+        <v>41353</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A25">
+        <v>-24</v>
+      </c>
+      <c r="B25">
+        <v>10</v>
+      </c>
+      <c r="D25" s="1">
+        <v>41353</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A26">
+        <v>-25</v>
+      </c>
+      <c r="B26">
+        <v>7</v>
+      </c>
+      <c r="D26" s="1">
+        <v>41353</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" copies="0"/>
+  <headerFooter alignWithMargins="0"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -4371,224 +4591,4 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H10"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="11.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="5.5703125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="6.42578125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="20.140625" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
-        <v>93</v>
-      </c>
-      <c r="B1" t="s">
-        <v>62</v>
-      </c>
-      <c r="C1" t="s">
-        <v>63</v>
-      </c>
-      <c r="D1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" t="s">
-        <v>17</v>
-      </c>
-      <c r="F1" t="s">
-        <v>20</v>
-      </c>
-      <c r="G1" t="s">
-        <v>19</v>
-      </c>
-      <c r="H1" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A2">
-        <v>-1</v>
-      </c>
-      <c r="B2">
-        <v>100</v>
-      </c>
-      <c r="C2">
-        <v>1</v>
-      </c>
-      <c r="D2">
-        <v>1000</v>
-      </c>
-      <c r="E2">
-        <v>5</v>
-      </c>
-      <c r="G2">
-        <v>-1</v>
-      </c>
-      <c r="H2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A3">
-        <v>-1</v>
-      </c>
-      <c r="C3">
-        <v>2</v>
-      </c>
-      <c r="D3">
-        <v>2000</v>
-      </c>
-      <c r="E3">
-        <v>3</v>
-      </c>
-      <c r="G3">
-        <v>-2</v>
-      </c>
-      <c r="H3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A4">
-        <v>-1</v>
-      </c>
-      <c r="C4">
-        <v>3</v>
-      </c>
-      <c r="D4">
-        <v>3000</v>
-      </c>
-      <c r="E4">
-        <v>4</v>
-      </c>
-      <c r="G4">
-        <v>-3</v>
-      </c>
-      <c r="H4">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A5">
-        <v>-2</v>
-      </c>
-      <c r="C5">
-        <v>4</v>
-      </c>
-      <c r="D5">
-        <v>1500</v>
-      </c>
-      <c r="E5">
-        <v>2</v>
-      </c>
-      <c r="G5">
-        <v>-1</v>
-      </c>
-      <c r="H5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A6">
-        <v>-3</v>
-      </c>
-      <c r="D6">
-        <v>1400</v>
-      </c>
-      <c r="E6">
-        <v>1</v>
-      </c>
-      <c r="G6">
-        <v>-2</v>
-      </c>
-      <c r="H6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A7">
-        <v>-4</v>
-      </c>
-      <c r="D7">
-        <v>2000</v>
-      </c>
-      <c r="E7">
-        <v>1</v>
-      </c>
-      <c r="G7">
-        <v>-3</v>
-      </c>
-      <c r="H7">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A8">
-        <v>-5</v>
-      </c>
-      <c r="D8">
-        <v>1900</v>
-      </c>
-      <c r="E8">
-        <v>2</v>
-      </c>
-      <c r="G8">
-        <v>-1</v>
-      </c>
-      <c r="H8">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A9">
-        <v>-6</v>
-      </c>
-      <c r="D9">
-        <v>1700</v>
-      </c>
-      <c r="E9">
-        <v>1</v>
-      </c>
-      <c r="G9">
-        <v>-1</v>
-      </c>
-      <c r="H9">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A10">
-        <v>-7</v>
-      </c>
-      <c r="D10">
-        <v>1800</v>
-      </c>
-      <c r="E10">
-        <v>1</v>
-      </c>
-      <c r="G10">
-        <v>-1</v>
-      </c>
-      <c r="H10">
-        <v>0</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-</worksheet>
 </file>
</xml_diff>